<commit_message>
Project_#RPA_Challenge code and deployment updated
code was updated
package and deployment excel sheet uploaded in SharePoint
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Lavanya/RPA Challenge_Code/Data/Config.xlsx
+++ b/SourceCode/2023/August2023/Lavanya/RPA Challenge_Code/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumanth\Documents\GitHub\RPA-Developer-in-30-Days\SourceCode\2023\August2023\Lavanya\RPA Challenge\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumanth\Documents\GitHub\RPA-Developer-in-30-Days\SourceCode\2023\August2023\Lavanya\RPA Challenge_Code\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F8C04-861F-4790-8EE2-78F8B0416BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0855854-4400-4802-A49A-22DB78023075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>